<commit_message>
Introducing UUID for COFI Hierarchy
First production run parameters in parameters.csv, results and source data excluded due to Data Privacy restrictions.
</commit_message>
<xml_diff>
--- a/Documentation/data_design.xlsx
+++ b/Documentation/data_design.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinfilip/Desktop/files/Python/Object Engine/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinfilip/Documents/GitHub/Object_Engine/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396753DC-5F53-254F-B6D1-7E563D30358B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8803E0-1AB5-594C-ADA0-42843FBE92AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16020" yWindow="0" windowWidth="26940" windowHeight="28800" activeTab="2" xr2:uid="{0C23F4B2-264A-4A41-89D4-667220E8A369}"/>
+    <workbookView xWindow="11460" yWindow="0" windowWidth="26940" windowHeight="21600" activeTab="2" xr2:uid="{0C23F4B2-264A-4A41-89D4-667220E8A369}"/>
   </bookViews>
   <sheets>
     <sheet name="object_engine.py" sheetId="7" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="87">
   <si>
     <t>batch_id</t>
   </si>
@@ -235,6 +235,69 @@
   </si>
   <si>
     <t>Customer name (directory name)</t>
+  </si>
+  <si>
+    <t>Customer Care</t>
+  </si>
+  <si>
+    <t>cases.csv</t>
+  </si>
+  <si>
+    <t>CaseNumber</t>
+  </si>
+  <si>
+    <t>C0000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>OI000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>FI000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>CreatedDate</t>
+  </si>
+  <si>
+    <t>FI000000000000000000000000000001</t>
+  </si>
+  <si>
+    <t>FI000000000000000000000000000002</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>FI000000000000000000000000000003</t>
+  </si>
+  <si>
+    <t>L1 Property</t>
+  </si>
+  <si>
+    <t>L1 Display Name</t>
+  </si>
+  <si>
+    <t>L2 Property</t>
+  </si>
+  <si>
+    <t>L2 Display Name</t>
+  </si>
+  <si>
+    <t>L3 Property</t>
+  </si>
+  <si>
+    <t>L3 Display Name</t>
+  </si>
+  <si>
+    <t>L1 Code</t>
+  </si>
+  <si>
+    <t>L2 Code</t>
+  </si>
+  <si>
+    <t>L3 Code</t>
+  </si>
+  <si>
+    <t>New</t>
   </si>
 </sst>
 </file>
@@ -361,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -376,6 +439,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -716,15 +780,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3931C615-53D1-A248-90B7-F35D751B2D75}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="41.33203125" customWidth="1"/>
+    <col min="1" max="12" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -848,6 +912,156 @@
         <v>54</v>
       </c>
       <c r="D12" s="6"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" t="s">
+        <v>70</v>
+      </c>
+      <c r="I17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" t="s">
+        <v>69</v>
+      </c>
+      <c r="H18" t="s">
+        <v>70</v>
+      </c>
+      <c r="I18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" t="s">
+        <v>69</v>
+      </c>
+      <c r="H19" t="s">
+        <v>70</v>
+      </c>
+      <c r="I19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" t="s">
+        <v>70</v>
+      </c>
+      <c r="I20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" t="s">
+        <v>82</v>
+      </c>
+      <c r="G22" t="s">
+        <v>83</v>
+      </c>
+      <c r="H22" t="s">
+        <v>84</v>
+      </c>
+      <c r="I22" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Structure & Design
Staging for multiple search functions and updated design doc to reflect.
</commit_message>
<xml_diff>
--- a/Documentation/data_design.xlsx
+++ b/Documentation/data_design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinfilip/Documents/GitHub/Object_Engine/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8803E0-1AB5-594C-ADA0-42843FBE92AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87510998-DE47-8943-96D5-A51C25FD0C5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11460" yWindow="0" windowWidth="26940" windowHeight="21600" activeTab="2" xr2:uid="{0C23F4B2-264A-4A41-89D4-667220E8A369}"/>
+    <workbookView xWindow="-9440" yWindow="-20900" windowWidth="36500" windowHeight="18620" activeTab="2" xr2:uid="{0C23F4B2-264A-4A41-89D4-667220E8A369}"/>
   </bookViews>
   <sheets>
     <sheet name="object_engine.py" sheetId="7" r:id="rId1"/>
@@ -18,8 +18,7 @@
     <sheet name="cofi" sheetId="1" r:id="rId3"/>
     <sheet name="parameters" sheetId="2" r:id="rId4"/>
     <sheet name="log" sheetId="4" r:id="rId5"/>
-    <sheet name="customers" sheetId="6" r:id="rId6"/>
-    <sheet name="results" sheetId="5" r:id="rId7"/>
+    <sheet name="results" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="91">
   <si>
     <t>batch_id</t>
   </si>
@@ -168,9 +167,6 @@
     <t>return_fields</t>
   </si>
   <si>
-    <t>This table identifies objects available for querying for the current customer directory</t>
-  </si>
-  <si>
     <t>Example contents of cofi file</t>
   </si>
   <si>
@@ -189,9 +185,6 @@
     <t>string</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
     <t>String (Object / file name)</t>
   </si>
   <si>
@@ -228,15 +221,6 @@
     <t>Contains the selected return fields for the selected object in a file named with a system timestamp for when the search completed, the Customer name, and the object name</t>
   </si>
   <si>
-    <t>Customer_Name_1</t>
-  </si>
-  <si>
-    <t>Customer_Name_2</t>
-  </si>
-  <si>
-    <t>Customer name (directory name)</t>
-  </si>
-  <si>
     <t>Customer Care</t>
   </si>
   <si>
@@ -297,14 +281,41 @@
     <t>L3 Code</t>
   </si>
   <si>
-    <t>New</t>
+    <t>search_method</t>
+  </si>
+  <si>
+    <t>Add this</t>
+  </si>
+  <si>
+    <t>customer_index</t>
+  </si>
+  <si>
+    <t>customer_name</t>
+  </si>
+  <si>
+    <t>customer_uuid</t>
+  </si>
+  <si>
+    <t>object_uuid</t>
+  </si>
+  <si>
+    <t>field_uuid</t>
+  </si>
+  <si>
+    <t>Anaplan List Hierarchy:</t>
+  </si>
+  <si>
+    <t>This table identifies customers, objects, fields, and search methods available for querying for the current customer directory</t>
+  </si>
+  <si>
+    <t>move this to first row instead of column?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -312,8 +323,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -344,8 +362,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -420,11 +444,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -437,9 +472,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -780,288 +818,451 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3931C615-53D1-A248-90B7-F35D751B2D75}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="12" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="45.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.5" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" customWidth="1"/>
+    <col min="8" max="10" width="33.5" customWidth="1"/>
+    <col min="11" max="13" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="4"/>
-      <c r="C1" s="3"/>
+      <c r="C1" s="4"/>
       <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="B2" s="4"/>
-      <c r="C2" s="3"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="3"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="H5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="12">
+        <v>0</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="12">
+        <v>0</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12">
+        <v>0</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="12">
+        <v>1</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12">
+        <v>0</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="12">
+        <v>2</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12">
+        <v>0</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="12">
+        <v>0</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="12">
+        <v>3</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="C15" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="C16" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="B17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>0</v>
-      </c>
-      <c r="B17" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17" t="s">
-        <v>68</v>
-      </c>
-      <c r="G17" t="s">
-        <v>69</v>
-      </c>
-      <c r="H17" t="s">
-        <v>70</v>
-      </c>
-      <c r="I17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>0</v>
-      </c>
-      <c r="B18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18" t="s">
-        <v>72</v>
-      </c>
-      <c r="G18" t="s">
-        <v>69</v>
-      </c>
-      <c r="H18" t="s">
-        <v>70</v>
-      </c>
-      <c r="I18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>0</v>
-      </c>
-      <c r="B19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19">
-        <v>2</v>
-      </c>
-      <c r="F19" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" t="s">
-        <v>69</v>
-      </c>
-      <c r="H19" t="s">
-        <v>70</v>
-      </c>
-      <c r="I19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>0</v>
-      </c>
-      <c r="B20" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20">
-        <v>3</v>
-      </c>
-      <c r="F20" t="s">
-        <v>75</v>
-      </c>
-      <c r="G20" t="s">
-        <v>69</v>
-      </c>
-      <c r="H20" t="s">
-        <v>70</v>
-      </c>
-      <c r="I20" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>77</v>
-      </c>
-      <c r="B22" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" t="s">
-        <v>79</v>
-      </c>
-      <c r="D22" t="s">
-        <v>80</v>
-      </c>
-      <c r="E22" t="s">
-        <v>81</v>
-      </c>
-      <c r="F22" t="s">
-        <v>82</v>
-      </c>
-      <c r="G22" t="s">
-        <v>83</v>
-      </c>
-      <c r="H22" t="s">
-        <v>84</v>
-      </c>
-      <c r="I22" t="s">
-        <v>85</v>
-      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1073,12 +1274,13 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="33.83203125" customWidth="1"/>
+    <col min="1" max="5" width="33.83203125" customWidth="1"/>
+    <col min="6" max="6" width="27" customWidth="1"/>
     <col min="7" max="8" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1091,6 +1293,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -1101,6 +1304,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1109,7 +1313,10 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="3"/>
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1129,6 +1336,9 @@
         <v>3</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="H4" s="5"/>
@@ -1150,6 +1360,9 @@
         <v>5</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="5"/>
@@ -1161,6 +1374,7 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1176,6 +1390,7 @@
       <c r="D7" s="4"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1185,6 +1400,7 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1200,6 +1416,7 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -1209,11 +1426,12 @@
         <v>41</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -1228,6 +1446,7 @@
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -1242,6 +1461,7 @@
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -1256,6 +1476,7 @@
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1559,53 +1780,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393971F4-79F2-8740-A53A-0EA43E9FC1FA}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="32" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF5E084-4BA9-9F4A-A02F-57E1CC126878}">
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1616,7 +1795,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1624,7 +1803,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1635,106 +1814,107 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
+      <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="3"/>
+      <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="3"/>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="3"/>
+      <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="12"/>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="13"/>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
@@ -1746,7 +1926,7 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="4"/>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
@@ -1758,7 +1938,7 @@
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
-      <c r="J10" s="3"/>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
@@ -1770,6 +1950,7 @@
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
@@ -1781,6 +1962,7 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
@@ -1792,6 +1974,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
@@ -1803,6 +1986,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
@@ -1814,6 +1998,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
@@ -1825,8 +2010,9 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1836,8 +2022,9 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1847,8 +2034,9 @@
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1859,7 +2047,7 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -1870,7 +2058,7 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1881,7 +2069,7 @@
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>

</xml_diff>

<commit_message>
Restructured for additional Methods
</commit_message>
<xml_diff>
--- a/Documentation/data_design.xlsx
+++ b/Documentation/data_design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinfilip/Documents/GitHub/Object_Engine/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87510998-DE47-8943-96D5-A51C25FD0C5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828D529A-8811-8641-8D70-63CA97CF5773}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9440" yWindow="-20900" windowWidth="36500" windowHeight="18620" activeTab="2" xr2:uid="{0C23F4B2-264A-4A41-89D4-667220E8A369}"/>
+    <workbookView xWindow="-9440" yWindow="-20900" windowWidth="36500" windowHeight="18620" activeTab="3" xr2:uid="{0C23F4B2-264A-4A41-89D4-667220E8A369}"/>
   </bookViews>
   <sheets>
     <sheet name="object_engine.py" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="93">
   <si>
     <t>batch_id</t>
   </si>
@@ -309,6 +309,12 @@
   </si>
   <si>
     <t>move this to first row instead of column?</t>
+  </si>
+  <si>
+    <t>selected_method</t>
+  </si>
+  <si>
+    <t>Int value representing the method to use against the data</t>
   </si>
 </sst>
 </file>
@@ -820,7 +826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3931C615-53D1-A248-90B7-F35D751B2D75}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
@@ -1271,10 +1277,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DE3BE6E-DEE3-9146-93D8-3606446DFF4F}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1284,7 +1290,7 @@
     <col min="7" max="8" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -1295,7 +1301,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -1307,7 +1313,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1319,55 +1325,61 @@
       <c r="G3" s="3"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1377,7 +1389,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1393,7 +1405,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1403,7 +1415,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
@@ -1418,65 +1430,80 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>1</v>
+        <v>91</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Minor Updates to Structure
</commit_message>
<xml_diff>
--- a/Documentation/data_design.xlsx
+++ b/Documentation/data_design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinfilip/Documents/GitHub/Object_Engine/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828D529A-8811-8641-8D70-63CA97CF5773}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC269AA8-E2F2-5649-A31A-36476328491B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9440" yWindow="-20900" windowWidth="36500" windowHeight="18620" activeTab="3" xr2:uid="{0C23F4B2-264A-4A41-89D4-667220E8A369}"/>
+    <workbookView xWindow="720" yWindow="0" windowWidth="36500" windowHeight="17500" activeTab="3" xr2:uid="{0C23F4B2-264A-4A41-89D4-667220E8A369}"/>
   </bookViews>
   <sheets>
     <sheet name="object_engine.py" sheetId="7" r:id="rId1"/>
@@ -827,7 +827,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1280,7 +1280,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1300,6 +1300,8 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -1311,7 +1313,8 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="5"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -1323,7 +1326,8 @@
         <v>82</v>
       </c>
       <c r="G3" s="3"/>
-      <c r="H3" s="5"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -1350,7 +1354,7 @@
       <c r="H4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="5"/>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -1377,7 +1381,7 @@
       <c r="H5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="5"/>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
@@ -1387,7 +1391,8 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="5"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -1403,7 +1408,8 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="5"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
@@ -1413,7 +1419,8 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="5"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -1429,6 +1436,8 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -1444,6 +1453,8 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -1459,6 +1470,8 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -1474,6 +1487,8 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -1489,6 +1504,8 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -1504,6 +1521,8 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Minor updates to keyword ranking
</commit_message>
<xml_diff>
--- a/Documentation/data_design.xlsx
+++ b/Documentation/data_design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinfilip/Documents/GitHub/Object_Engine/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC269AA8-E2F2-5649-A31A-36476328491B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372DAA73-7D17-2244-ACD4-4E9D60CB0528}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="0" windowWidth="36500" windowHeight="17500" activeTab="3" xr2:uid="{0C23F4B2-264A-4A41-89D4-667220E8A369}"/>
+    <workbookView xWindow="16840" yWindow="20" windowWidth="21540" windowHeight="10260" activeTab="5" xr2:uid="{0C23F4B2-264A-4A41-89D4-667220E8A369}"/>
   </bookViews>
   <sheets>
     <sheet name="object_engine.py" sheetId="7" r:id="rId1"/>
@@ -28,7 +28,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="99">
   <si>
     <t>batch_id</t>
   </si>
@@ -200,12 +202,6 @@
     <t xml:space="preserve">Int value representing the object(s) to execute the search on, used for chunking large amounts of data into smaller searches against subsets of data. (Ex: x Time) </t>
   </si>
   <si>
-    <t>first selected field for object</t>
-  </si>
-  <si>
-    <t>any other selected fields ---&gt;&gt;</t>
-  </si>
-  <si>
     <t>---&gt;&gt;</t>
   </si>
   <si>
@@ -315,6 +311,30 @@
   </si>
   <si>
     <t>Int value representing the method to use against the data</t>
+  </si>
+  <si>
+    <t>For Method 0 - Match String or RegEx against specified field.</t>
+  </si>
+  <si>
+    <t>Top 5 Ranked Named Entities for specified field</t>
+  </si>
+  <si>
+    <t>For Method 1 - Keyword Ranking against specified field for Named Entities.</t>
+  </si>
+  <si>
+    <t>field contents</t>
+  </si>
+  <si>
+    <t>First selected return field for object</t>
+  </si>
+  <si>
+    <t>Other specified return fields, in order as entered ---&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">---&gt;&gt; etc.. </t>
+  </si>
+  <si>
+    <t>etc..</t>
   </si>
 </sst>
 </file>
@@ -465,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -484,6 +504,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -860,7 +881,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -888,46 +909,46 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B4" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="E4" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="F4" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="G4" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="H4" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="I4" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="J4" s="17" t="s">
         <v>78</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>80</v>
       </c>
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>44</v>
@@ -942,46 +963,46 @@
         <v>47</v>
       </c>
       <c r="H5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B6" s="12">
         <v>0</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D6" s="12">
         <v>0</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F6" s="12">
         <v>0</v>
       </c>
       <c r="G6" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="J6" s="12" t="s">
         <v>64</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>66</v>
       </c>
       <c r="K6" s="4"/>
     </row>
@@ -991,28 +1012,28 @@
         <v>0</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D7" s="12">
         <v>0</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F7" s="12">
         <v>1</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K7" s="4"/>
     </row>
@@ -1022,13 +1043,13 @@
         <v>0</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D8" s="12">
         <v>0</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F8" s="12">
         <v>2</v>
@@ -1037,13 +1058,13 @@
         <v>24</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K8" s="4"/>
     </row>
@@ -1053,28 +1074,28 @@
         <v>0</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D9" s="12">
         <v>0</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F9" s="12">
         <v>3</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K9" s="4"/>
     </row>
@@ -1093,7 +1114,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="13"/>
@@ -1108,7 +1129,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="13"/>
@@ -1123,7 +1144,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="13"/>
@@ -1214,7 +1235,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="13"/>
@@ -1229,7 +1250,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="13"/>
@@ -1244,7 +1265,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="13"/>
@@ -1279,8 +1300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DE3BE6E-DEE3-9146-93D8-3606446DFF4F}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1323,7 +1344,7 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -1334,7 +1355,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>1</v>
@@ -1349,7 +1370,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>4</v>
@@ -1441,13 +1462,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -1827,154 +1848,164 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF5E084-4BA9-9F4A-A02F-57E1CC126878}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="37.83203125" customWidth="1"/>
-    <col min="5" max="10" width="25.5" customWidth="1"/>
+    <col min="1" max="1" width="37.83203125" customWidth="1"/>
+    <col min="2" max="2" width="50" customWidth="1"/>
+    <col min="3" max="3" width="37.83203125" customWidth="1"/>
+    <col min="4" max="4" width="40.83203125" customWidth="1"/>
+    <col min="5" max="5" width="41.6640625" customWidth="1"/>
+    <col min="6" max="10" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="5"/>
+      <c r="D5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="5"/>
+        <v>56</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="5"/>
+        <v>55</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="5"/>
+        <v>55</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1986,77 +2017,135 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>94</v>
+      </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="K13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
@@ -2092,6 +2181,7 @@
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
@@ -2126,6 +2216,22 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
     </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>